<commit_message>
Changed author of documents
</commit_message>
<xml_diff>
--- a/PR/Week04_PR_F14a_T01.xlsx
+++ b/PR/Week04_PR_F14a_T01.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echo\Documents\GitHub\We-are-Trojans\WeAreTrojan\PR\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="15615" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SLOC" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,7 @@
     <sheet name="COTS" sheetId="4" r:id="rId4"/>
     <sheet name="Defects, Problems, and Concerns" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1731,27 +1736,9 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1767,34 +1754,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1807,14 +1766,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1837,34 +1788,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1874,19 +1797,109 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2216,14 +2229,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" customWidth="1"/>
-    <col min="3" max="13" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="13" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" customHeight="1">
+    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2238,7 +2251,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1">
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -2257,7 +2270,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="15" customHeight="1">
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -2276,7 +2289,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1">
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
@@ -2291,7 +2304,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" ht="15" customHeight="1">
+    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2306,7 +2319,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="15" customHeight="1">
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2321,7 +2334,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" ht="15" customHeight="1">
+    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="7" t="s">
         <v>2</v>
@@ -2340,7 +2353,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1">
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="8" t="s">
         <v>4</v>
@@ -2359,7 +2372,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1">
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="9" t="s">
         <v>5</v>
@@ -2378,7 +2391,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" ht="15" customHeight="1">
+    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="9" t="s">
         <v>6</v>
@@ -2397,7 +2410,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" ht="15" customHeight="1">
+    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="9" t="s">
         <v>7</v>
@@ -2416,7 +2429,7 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" ht="15" customHeight="1">
+    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="9" t="s">
         <v>8</v>
@@ -2435,7 +2448,7 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" ht="15" customHeight="1">
+    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="9" t="s">
         <v>9</v>
@@ -2454,7 +2467,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" ht="15" customHeight="1">
+    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="5" t="s">
         <v>10</v>
@@ -2473,7 +2486,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" ht="15" customHeight="1">
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2488,7 +2501,7 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" ht="15" customHeight="1">
+    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2503,7 +2516,7 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1">
+    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2518,7 +2531,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1">
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2533,7 +2546,7 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1">
+    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2548,7 +2561,7 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" ht="15" customHeight="1">
+    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2581,19 +2594,19 @@
       <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" customWidth="1"/>
-    <col min="2" max="2" width="2.1640625" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="2.140625" customWidth="1"/>
     <col min="3" max="3" width="40" customWidth="1"/>
-    <col min="4" max="4" width="11.5" customWidth="1"/>
-    <col min="5" max="5" width="3.6640625" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" customWidth="1"/>
-    <col min="7" max="7" width="43.83203125" customWidth="1"/>
-    <col min="8" max="16" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="43.85546875" customWidth="1"/>
+    <col min="8" max="16" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="12" customHeight="1">
+    <row r="1" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2611,7 +2624,7 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:16" ht="15.75" customHeight="1">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="10" t="s">
         <v>11</v>
@@ -2631,7 +2644,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="12" customHeight="1">
+    <row r="3" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="5" t="s">
         <v>12</v>
@@ -2651,7 +2664,7 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1">
+    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2669,7 +2682,7 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" ht="12" customHeight="1" thickBot="1">
+    <row r="5" spans="1:16" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2687,18 +2700,18 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" ht="22" customHeight="1" thickBot="1">
+    <row r="6" spans="1:16" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="144" t="s">
+      <c r="B6" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="145" t="s">
+      <c r="C6" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="146"/>
-      <c r="E6" s="146"/>
-      <c r="F6" s="146"/>
-      <c r="G6" s="147"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="105"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -2709,18 +2722,18 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" ht="12" customHeight="1">
+    <row r="7" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="148">
+      <c r="B7" s="106">
         <v>1</v>
       </c>
-      <c r="C7" s="143" t="s">
+      <c r="C7" s="110" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="107"/>
-      <c r="E7" s="107"/>
-      <c r="F7" s="107"/>
-      <c r="G7" s="97"/>
+      <c r="D7" s="111"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="111"/>
+      <c r="G7" s="112"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -2731,19 +2744,19 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" ht="12" customHeight="1">
+    <row r="8" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="149">
+      <c r="B8" s="107">
         <f t="shared" ref="B8:B14" si="0">B7+1</f>
         <v>2</v>
       </c>
-      <c r="C8" s="143" t="s">
+      <c r="C8" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="107"/>
-      <c r="E8" s="107"/>
-      <c r="F8" s="107"/>
-      <c r="G8" s="97"/>
+      <c r="D8" s="111"/>
+      <c r="E8" s="111"/>
+      <c r="F8" s="111"/>
+      <c r="G8" s="112"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -2754,19 +2767,19 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" ht="12" customHeight="1">
+    <row r="9" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="149">
+      <c r="B9" s="107">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C9" s="143" t="s">
+      <c r="C9" s="110" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="107"/>
-      <c r="E9" s="107"/>
-      <c r="F9" s="107"/>
-      <c r="G9" s="97"/>
+      <c r="D9" s="111"/>
+      <c r="E9" s="111"/>
+      <c r="F9" s="111"/>
+      <c r="G9" s="112"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -2777,19 +2790,19 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" ht="12" customHeight="1">
+    <row r="10" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="149">
+      <c r="B10" s="107">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C10" s="143" t="s">
+      <c r="C10" s="110" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="107"/>
-      <c r="E10" s="107"/>
-      <c r="F10" s="107"/>
-      <c r="G10" s="97"/>
+      <c r="D10" s="111"/>
+      <c r="E10" s="111"/>
+      <c r="F10" s="111"/>
+      <c r="G10" s="112"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -2800,19 +2813,19 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" ht="12" customHeight="1">
+    <row r="11" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="149">
+      <c r="B11" s="107">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C11" s="143" t="s">
+      <c r="C11" s="110" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="107"/>
-      <c r="E11" s="107"/>
-      <c r="F11" s="107"/>
-      <c r="G11" s="97"/>
+      <c r="D11" s="111"/>
+      <c r="E11" s="111"/>
+      <c r="F11" s="111"/>
+      <c r="G11" s="112"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -2823,19 +2836,19 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" ht="12" customHeight="1">
+    <row r="12" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="149">
+      <c r="B12" s="107">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C12" s="143" t="s">
+      <c r="C12" s="110" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="107"/>
-      <c r="E12" s="107"/>
-      <c r="F12" s="107"/>
-      <c r="G12" s="97"/>
+      <c r="D12" s="111"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="111"/>
+      <c r="G12" s="112"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -2846,19 +2859,19 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" ht="12" customHeight="1">
+    <row r="13" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="149">
+      <c r="B13" s="107">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C13" s="143" t="s">
+      <c r="C13" s="110" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="107"/>
-      <c r="E13" s="107"/>
-      <c r="F13" s="107"/>
-      <c r="G13" s="97"/>
+      <c r="D13" s="111"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="111"/>
+      <c r="G13" s="112"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -2869,17 +2882,17 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" ht="12.75" customHeight="1" thickBot="1">
+    <row r="14" spans="1:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="150">
+      <c r="B14" s="108">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C14" s="151"/>
-      <c r="D14" s="132"/>
-      <c r="E14" s="132"/>
-      <c r="F14" s="132"/>
-      <c r="G14" s="103"/>
+      <c r="C14" s="116"/>
+      <c r="D14" s="114"/>
+      <c r="E14" s="114"/>
+      <c r="F14" s="114"/>
+      <c r="G14" s="115"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -2890,7 +2903,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" ht="22" customHeight="1" thickBot="1">
+    <row r="15" spans="1:16" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2908,18 +2921,18 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" ht="20" customHeight="1" thickBot="1">
+    <row r="16" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="B16" s="144" t="s">
+      <c r="B16" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="145" t="s">
+      <c r="C16" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="146"/>
-      <c r="E16" s="146"/>
-      <c r="F16" s="146"/>
-      <c r="G16" s="147"/>
+      <c r="D16" s="104"/>
+      <c r="E16" s="104"/>
+      <c r="F16" s="104"/>
+      <c r="G16" s="105"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -2930,18 +2943,18 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" ht="12" customHeight="1">
+    <row r="17" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="148">
+      <c r="B17" s="106">
         <v>1</v>
       </c>
-      <c r="C17" s="143" t="s">
+      <c r="C17" s="110" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="107"/>
-      <c r="E17" s="107"/>
-      <c r="F17" s="107"/>
-      <c r="G17" s="97"/>
+      <c r="D17" s="111"/>
+      <c r="E17" s="111"/>
+      <c r="F17" s="111"/>
+      <c r="G17" s="112"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -2952,19 +2965,19 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16" ht="12" customHeight="1">
+    <row r="18" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="149">
+      <c r="B18" s="107">
         <f>B17+1</f>
         <v>2</v>
       </c>
-      <c r="C18" s="143" t="s">
+      <c r="C18" s="110" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="107"/>
-      <c r="E18" s="107"/>
-      <c r="F18" s="107"/>
-      <c r="G18" s="97"/>
+      <c r="D18" s="111"/>
+      <c r="E18" s="111"/>
+      <c r="F18" s="111"/>
+      <c r="G18" s="112"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -2975,19 +2988,19 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" ht="12" customHeight="1">
+    <row r="19" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="149">
+      <c r="B19" s="107">
         <f>B18+1</f>
         <v>3</v>
       </c>
-      <c r="C19" s="143" t="s">
+      <c r="C19" s="110" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="107"/>
-      <c r="E19" s="107"/>
-      <c r="F19" s="107"/>
-      <c r="G19" s="97"/>
+      <c r="D19" s="111"/>
+      <c r="E19" s="111"/>
+      <c r="F19" s="111"/>
+      <c r="G19" s="112"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -2998,17 +3011,17 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:16" ht="12" customHeight="1">
+    <row r="20" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="149">
+      <c r="B20" s="107">
         <f>B19+1</f>
         <v>4</v>
       </c>
-      <c r="C20" s="143"/>
-      <c r="D20" s="107"/>
-      <c r="E20" s="107"/>
-      <c r="F20" s="107"/>
-      <c r="G20" s="97"/>
+      <c r="C20" s="110"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="111"/>
+      <c r="F20" s="111"/>
+      <c r="G20" s="112"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -3019,19 +3032,19 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" ht="12.75" customHeight="1" thickBot="1">
+    <row r="21" spans="1:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="150">
+      <c r="B21" s="108">
         <f>B20+1</f>
         <v>5</v>
       </c>
-      <c r="C21" s="152" t="s">
+      <c r="C21" s="113" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="132"/>
-      <c r="E21" s="132"/>
-      <c r="F21" s="132"/>
-      <c r="G21" s="103"/>
+      <c r="D21" s="114"/>
+      <c r="E21" s="114"/>
+      <c r="F21" s="114"/>
+      <c r="G21" s="115"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -3042,7 +3055,7 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16" ht="12" customHeight="1" thickBot="1">
+    <row r="22" spans="1:16" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -3060,18 +3073,18 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="1:16" ht="12.75" customHeight="1" thickBot="1">
+    <row r="23" spans="1:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="144" t="s">
+      <c r="B23" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="145" t="s">
+      <c r="C23" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="146"/>
-      <c r="E23" s="146"/>
-      <c r="F23" s="153"/>
-      <c r="G23" s="147"/>
+      <c r="D23" s="104"/>
+      <c r="E23" s="104"/>
+      <c r="F23" s="109"/>
+      <c r="G23" s="105"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -3082,18 +3095,18 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="1:16" ht="15" customHeight="1">
+    <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="148">
+      <c r="B24" s="106">
         <v>1</v>
       </c>
-      <c r="C24" s="143" t="s">
+      <c r="C24" s="110" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="107"/>
-      <c r="E24" s="107"/>
-      <c r="F24" s="107"/>
-      <c r="G24" s="97"/>
+      <c r="D24" s="111"/>
+      <c r="E24" s="111"/>
+      <c r="F24" s="111"/>
+      <c r="G24" s="112"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -3104,19 +3117,19 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="1:16" ht="12" customHeight="1">
+    <row r="25" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="149">
+      <c r="B25" s="107">
         <f t="shared" ref="B25:B31" si="1">B24+1</f>
         <v>2</v>
       </c>
-      <c r="C25" s="143" t="s">
+      <c r="C25" s="110" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="107"/>
-      <c r="E25" s="107"/>
-      <c r="F25" s="107"/>
-      <c r="G25" s="97"/>
+      <c r="D25" s="111"/>
+      <c r="E25" s="111"/>
+      <c r="F25" s="111"/>
+      <c r="G25" s="112"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -3127,19 +3140,19 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16" ht="12" customHeight="1">
+    <row r="26" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="149">
+      <c r="B26" s="107">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="C26" s="143" t="s">
+      <c r="C26" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="107"/>
-      <c r="E26" s="107"/>
-      <c r="F26" s="107"/>
-      <c r="G26" s="97"/>
+      <c r="D26" s="111"/>
+      <c r="E26" s="111"/>
+      <c r="F26" s="111"/>
+      <c r="G26" s="112"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -3150,19 +3163,19 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="1:16" ht="12" customHeight="1">
+    <row r="27" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="149">
+      <c r="B27" s="107">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="C27" s="143" t="s">
+      <c r="C27" s="110" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="107"/>
-      <c r="E27" s="107"/>
-      <c r="F27" s="107"/>
-      <c r="G27" s="97"/>
+      <c r="D27" s="111"/>
+      <c r="E27" s="111"/>
+      <c r="F27" s="111"/>
+      <c r="G27" s="112"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -3173,19 +3186,19 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="1:16" ht="12" customHeight="1">
+    <row r="28" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="149">
+      <c r="B28" s="107">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="C28" s="143" t="s">
+      <c r="C28" s="110" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="107"/>
-      <c r="E28" s="107"/>
-      <c r="F28" s="107"/>
-      <c r="G28" s="97"/>
+      <c r="D28" s="111"/>
+      <c r="E28" s="111"/>
+      <c r="F28" s="111"/>
+      <c r="G28" s="112"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -3196,19 +3209,19 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="1:16" ht="12" customHeight="1">
+    <row r="29" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="149">
+      <c r="B29" s="107">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="C29" s="143" t="s">
+      <c r="C29" s="110" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="107"/>
-      <c r="E29" s="107"/>
-      <c r="F29" s="107"/>
-      <c r="G29" s="97"/>
+      <c r="D29" s="111"/>
+      <c r="E29" s="111"/>
+      <c r="F29" s="111"/>
+      <c r="G29" s="112"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -3219,19 +3232,19 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="1:16" ht="12" customHeight="1">
+    <row r="30" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="149">
+      <c r="B30" s="107">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="C30" s="143" t="s">
+      <c r="C30" s="110" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="107"/>
-      <c r="E30" s="107"/>
-      <c r="F30" s="107"/>
-      <c r="G30" s="97"/>
+      <c r="D30" s="111"/>
+      <c r="E30" s="111"/>
+      <c r="F30" s="111"/>
+      <c r="G30" s="112"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -3242,17 +3255,17 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16" ht="12.75" customHeight="1" thickBot="1">
+    <row r="31" spans="1:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
-      <c r="B31" s="150">
+      <c r="B31" s="108">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="C31" s="152"/>
-      <c r="D31" s="132"/>
-      <c r="E31" s="132"/>
-      <c r="F31" s="132"/>
-      <c r="G31" s="103"/>
+      <c r="C31" s="113"/>
+      <c r="D31" s="114"/>
+      <c r="E31" s="114"/>
+      <c r="F31" s="114"/>
+      <c r="G31" s="115"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -3263,7 +3276,7 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="1:16" ht="12" customHeight="1">
+    <row r="32" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -3281,7 +3294,7 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="1:16" ht="12" customHeight="1">
+    <row r="33" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -3299,7 +3312,7 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="1:16" ht="12" customHeight="1">
+    <row r="34" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="12" t="s">
         <v>37</v>
@@ -3321,7 +3334,7 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="1:16" ht="12" customHeight="1">
+    <row r="35" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -3339,7 +3352,7 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
     </row>
-    <row r="36" spans="1:16" ht="12" customHeight="1">
+    <row r="36" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="14" t="s">
@@ -3363,7 +3376,7 @@
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="1:16" ht="12" customHeight="1">
+    <row r="37" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="5" t="s">
@@ -3388,7 +3401,7 @@
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
     </row>
-    <row r="38" spans="1:16" ht="12" customHeight="1">
+    <row r="38" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="5" t="s">
@@ -3413,7 +3426,7 @@
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
     </row>
-    <row r="39" spans="1:16" ht="12" customHeight="1">
+    <row r="39" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="5" t="s">
@@ -3437,7 +3450,7 @@
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
     </row>
-    <row r="40" spans="1:16" ht="12" customHeight="1">
+    <row r="40" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="5" t="s">
@@ -3461,7 +3474,7 @@
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
     </row>
-    <row r="41" spans="1:16" ht="12" customHeight="1">
+    <row r="41" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="5" t="s">
@@ -3485,7 +3498,7 @@
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
     </row>
-    <row r="42" spans="1:16" ht="12" customHeight="1">
+    <row r="42" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="5" t="s">
@@ -3509,7 +3522,7 @@
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
     </row>
-    <row r="43" spans="1:16" ht="12" customHeight="1">
+    <row r="43" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="5" t="s">
@@ -3533,7 +3546,7 @@
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
     </row>
-    <row r="44" spans="1:16" ht="12" customHeight="1">
+    <row r="44" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="5" t="s">
@@ -3557,7 +3570,7 @@
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
     </row>
-    <row r="45" spans="1:16" ht="12" customHeight="1">
+    <row r="45" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="5" t="s">
@@ -3582,7 +3595,7 @@
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
     </row>
-    <row r="46" spans="1:16" ht="12" customHeight="1">
+    <row r="46" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -3600,7 +3613,7 @@
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
     </row>
-    <row r="47" spans="1:16" ht="12" customHeight="1">
+    <row r="47" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -3618,7 +3631,7 @@
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
     </row>
-    <row r="48" spans="1:16" ht="12" customHeight="1">
+    <row r="48" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -3636,7 +3649,7 @@
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
     </row>
-    <row r="49" spans="1:16" ht="12" customHeight="1">
+    <row r="49" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -3654,7 +3667,7 @@
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
     </row>
-    <row r="50" spans="1:16" ht="12" customHeight="1">
+    <row r="50" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -3672,7 +3685,7 @@
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
     </row>
-    <row r="51" spans="1:16" ht="12" customHeight="1">
+    <row r="51" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -3690,7 +3703,7 @@
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
     </row>
-    <row r="52" spans="1:16" ht="12" customHeight="1">
+    <row r="52" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -3708,7 +3721,7 @@
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
     </row>
-    <row r="53" spans="1:16" ht="12" customHeight="1">
+    <row r="53" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -3726,7 +3739,7 @@
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
     </row>
-    <row r="54" spans="1:16" ht="12" customHeight="1">
+    <row r="54" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -3744,7 +3757,7 @@
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
     </row>
-    <row r="55" spans="1:16" ht="12" customHeight="1">
+    <row r="55" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -3762,7 +3775,7 @@
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
     </row>
-    <row r="56" spans="1:16" ht="12" customHeight="1">
+    <row r="56" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -3780,7 +3793,7 @@
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
     </row>
-    <row r="57" spans="1:16" ht="12" customHeight="1">
+    <row r="57" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -3798,7 +3811,7 @@
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
     </row>
-    <row r="58" spans="1:16" ht="12" customHeight="1">
+    <row r="58" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -3816,7 +3829,7 @@
       <c r="O58" s="1"/>
       <c r="P58" s="1"/>
     </row>
-    <row r="59" spans="1:16" ht="12" customHeight="1">
+    <row r="59" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -3834,7 +3847,7 @@
       <c r="O59" s="1"/>
       <c r="P59" s="1"/>
     </row>
-    <row r="60" spans="1:16" ht="12" customHeight="1">
+    <row r="60" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -3852,7 +3865,7 @@
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
     </row>
-    <row r="61" spans="1:16" ht="12" customHeight="1">
+    <row r="61" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -3870,7 +3883,7 @@
       <c r="O61" s="1"/>
       <c r="P61" s="1"/>
     </row>
-    <row r="62" spans="1:16" ht="12" customHeight="1">
+    <row r="62" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -3888,7 +3901,7 @@
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
     </row>
-    <row r="63" spans="1:16" ht="12" customHeight="1">
+    <row r="63" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -3906,7 +3919,7 @@
       <c r="O63" s="1"/>
       <c r="P63" s="1"/>
     </row>
-    <row r="64" spans="1:16" ht="12" customHeight="1">
+    <row r="64" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -3924,7 +3937,7 @@
       <c r="O64" s="1"/>
       <c r="P64" s="1"/>
     </row>
-    <row r="65" spans="1:16" ht="12" customHeight="1">
+    <row r="65" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -3942,7 +3955,7 @@
       <c r="O65" s="1"/>
       <c r="P65" s="1"/>
     </row>
-    <row r="66" spans="1:16" ht="12" customHeight="1">
+    <row r="66" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -3962,11 +3975,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C17:G17"/>
     <mergeCell ref="C18:G18"/>
     <mergeCell ref="C28:G28"/>
     <mergeCell ref="C30:G30"/>
@@ -3977,12 +3985,17 @@
     <mergeCell ref="C24:G24"/>
     <mergeCell ref="C25:G25"/>
     <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C17:G17"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C13:G13"/>
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C19:G19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -4001,17 +4014,17 @@
       <selection activeCell="D5" sqref="D5:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.5" customWidth="1"/>
-    <col min="2" max="3" width="5.6640625" customWidth="1"/>
-    <col min="4" max="4" width="43.5" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" customWidth="1"/>
-    <col min="6" max="8" width="7.83203125" customWidth="1"/>
-    <col min="9" max="19" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="3" width="5.7109375" customWidth="1"/>
+    <col min="4" max="4" width="43.42578125" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" customWidth="1"/>
+    <col min="6" max="8" width="7.85546875" customWidth="1"/>
+    <col min="9" max="19" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" customHeight="1">
+    <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4032,18 +4045,18 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="140" t="s">
+      <c r="B2" s="117" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141"/>
-      <c r="E2" s="141"/>
-      <c r="F2" s="141"/>
-      <c r="G2" s="141"/>
-      <c r="H2" s="141"/>
-      <c r="I2" s="87"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="119"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -4055,16 +4068,16 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="142"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="106"/>
-      <c r="G3" s="106"/>
-      <c r="H3" s="106"/>
-      <c r="I3" s="88"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="121"/>
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="122"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -4076,16 +4089,16 @@
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="1:19" ht="15" customHeight="1">
+    <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="135"/>
-      <c r="C4" s="136"/>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="136"/>
-      <c r="H4" s="136"/>
-      <c r="I4" s="137"/>
+      <c r="B4" s="123"/>
+      <c r="C4" s="124"/>
+      <c r="D4" s="124"/>
+      <c r="E4" s="124"/>
+      <c r="F4" s="124"/>
+      <c r="G4" s="124"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="125"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -4097,28 +4110,28 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:19" ht="15" customHeight="1">
+    <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="79" t="s">
+      <c r="B5" s="126" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="80" t="s">
+      <c r="C5" s="127"/>
+      <c r="D5" s="128" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="133" t="s">
+      <c r="E5" s="129" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="138" t="s">
+      <c r="F5" s="131" t="s">
         <v>55</v>
       </c>
-      <c r="G5" s="138" t="s">
+      <c r="G5" s="131" t="s">
         <v>56</v>
       </c>
-      <c r="H5" s="138" t="s">
+      <c r="H5" s="131" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="134" t="s">
+      <c r="I5" s="130" t="s">
         <v>58</v>
       </c>
       <c r="J5" s="1"/>
@@ -4132,7 +4145,7 @@
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:19" ht="24" customHeight="1">
+    <row r="6" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="18" t="s">
         <v>59</v>
@@ -4140,12 +4153,12 @@
       <c r="C6" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="78"/>
-      <c r="E6" s="135"/>
-      <c r="F6" s="139"/>
-      <c r="G6" s="139"/>
-      <c r="H6" s="139"/>
-      <c r="I6" s="137"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="132"/>
+      <c r="H6" s="132"/>
+      <c r="I6" s="125"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -4157,7 +4170,7 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:19" ht="57" customHeight="1">
+    <row r="7" spans="1:19" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="19">
         <v>1</v>
@@ -4168,7 +4181,7 @@
       <c r="D7" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="86" t="s">
+      <c r="E7" s="78" t="s">
         <v>62</v>
       </c>
       <c r="F7" s="21">
@@ -4194,7 +4207,7 @@
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="1:19" ht="78" customHeight="1">
+    <row r="8" spans="1:19" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="19">
         <f t="shared" ref="B8:B16" si="1">B7+1</f>
@@ -4228,7 +4241,7 @@
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
     </row>
-    <row r="9" spans="1:19" ht="108" customHeight="1">
+    <row r="9" spans="1:19" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="19">
         <f t="shared" si="1"/>
@@ -4262,7 +4275,7 @@
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
     </row>
-    <row r="10" spans="1:19" ht="81" customHeight="1">
+    <row r="10" spans="1:19" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="19">
         <f t="shared" si="1"/>
@@ -4297,7 +4310,7 @@
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
     </row>
-    <row r="11" spans="1:19" ht="52" customHeight="1">
+    <row r="11" spans="1:19" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="19">
         <f t="shared" si="1"/>
@@ -4331,7 +4344,7 @@
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
     </row>
-    <row r="12" spans="1:19" ht="69" customHeight="1">
+    <row r="12" spans="1:19" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="19">
         <f t="shared" si="1"/>
@@ -4370,7 +4383,7 @@
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="1:19" ht="65" customHeight="1">
+    <row r="13" spans="1:19" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="19">
         <f t="shared" si="1"/>
@@ -4409,7 +4422,7 @@
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="1:19" ht="26.25" customHeight="1">
+    <row r="14" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="19">
         <f t="shared" si="1"/>
@@ -4434,7 +4447,7 @@
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
     </row>
-    <row r="15" spans="1:19" ht="26.25" customHeight="1">
+    <row r="15" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="19">
         <f t="shared" si="1"/>
@@ -4459,7 +4472,7 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:19" ht="26.25" customHeight="1">
+    <row r="16" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="19">
         <f t="shared" si="1"/>
@@ -4485,7 +4498,7 @@
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1">
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -4506,7 +4519,7 @@
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
     </row>
-    <row r="18" spans="1:19" ht="15" customHeight="1">
+    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -4527,7 +4540,7 @@
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
     </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1">
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -4548,7 +4561,7 @@
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
     </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1">
+    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -4597,20 +4610,20 @@
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="29.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="29.83203125" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" customWidth="1"/>
     <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" customWidth="1"/>
     <col min="8" max="8" width="7" customWidth="1"/>
-    <col min="9" max="18" width="8.83203125" customWidth="1"/>
+    <col min="9" max="18" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" customHeight="1">
+    <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4630,17 +4643,17 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:18" ht="15" customHeight="1">
+    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="141" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="127"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -4652,7 +4665,7 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
+    <row r="3" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4672,23 +4685,23 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="25.5" customHeight="1" thickBot="1">
+    <row r="4" spans="1:18" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="34"/>
-      <c r="B4" s="118" t="s">
+      <c r="B4" s="90" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="119" t="s">
+      <c r="C4" s="91" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="112" t="s">
+      <c r="D4" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="113"/>
-      <c r="F4" s="114" t="s">
+      <c r="E4" s="138"/>
+      <c r="F4" s="139" t="s">
         <v>83</v>
       </c>
-      <c r="G4" s="113"/>
-      <c r="H4" s="115"/>
+      <c r="G4" s="138"/>
+      <c r="H4" s="140"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -4700,23 +4713,23 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" ht="26.25" customHeight="1">
+    <row r="5" spans="1:18" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="116"/>
-      <c r="C5" s="117"/>
-      <c r="D5" s="108" t="s">
+      <c r="B5" s="88"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="109" t="s">
+      <c r="E5" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="F5" s="110" t="s">
+      <c r="F5" s="86" t="s">
         <v>86</v>
       </c>
-      <c r="G5" s="110" t="s">
+      <c r="G5" s="86" t="s">
         <v>87</v>
       </c>
-      <c r="H5" s="111" t="s">
+      <c r="H5" s="87" t="s">
         <v>88</v>
       </c>
       <c r="I5" s="1"/>
@@ -4730,7 +4743,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" ht="45" customHeight="1">
+    <row r="6" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="35"/>
       <c r="B6" s="36" t="s">
         <v>89</v>
@@ -4758,7 +4771,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" ht="15" customHeight="1">
+    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="43" t="s">
         <v>93</v>
@@ -4784,7 +4797,7 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" ht="15" customHeight="1">
+    <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="43" t="s">
         <v>96</v>
@@ -4812,7 +4825,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" ht="15" customHeight="1">
+    <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="49" t="s">
         <v>100</v>
@@ -4840,7 +4853,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" ht="15" customHeight="1">
+    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="49" t="s">
         <v>104</v>
@@ -4868,7 +4881,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" ht="15" customHeight="1">
+    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="49" t="s">
         <v>108</v>
@@ -4896,7 +4909,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" ht="15.75" customHeight="1">
+    <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="53" t="s">
         <v>112</v>
@@ -4924,7 +4937,7 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1">
+    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="57"/>
       <c r="C13" s="57"/>
@@ -4944,7 +4957,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" ht="15" customHeight="1">
+    <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="58"/>
       <c r="C14" s="58"/>
@@ -4964,17 +4977,17 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" ht="15.75" customHeight="1">
+    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="141" t="s">
         <v>116</v>
       </c>
-      <c r="C15" s="78"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="78"/>
+      <c r="C15" s="127"/>
+      <c r="D15" s="127"/>
+      <c r="E15" s="127"/>
+      <c r="F15" s="127"/>
+      <c r="G15" s="127"/>
+      <c r="H15" s="127"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -4986,7 +4999,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
+    <row r="16" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="59"/>
       <c r="C16" s="59"/>
@@ -5006,21 +5019,21 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18" ht="51" customHeight="1">
+    <row r="17" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="89" t="s">
+      <c r="B17" s="79" t="s">
         <v>117</v>
       </c>
-      <c r="C17" s="94" t="s">
+      <c r="C17" s="133" t="s">
         <v>118</v>
       </c>
-      <c r="D17" s="95"/>
-      <c r="E17" s="104" t="s">
+      <c r="D17" s="134"/>
+      <c r="E17" s="135" t="s">
         <v>119</v>
       </c>
-      <c r="F17" s="105"/>
-      <c r="G17" s="105"/>
-      <c r="H17" s="95"/>
+      <c r="F17" s="136"/>
+      <c r="G17" s="136"/>
+      <c r="H17" s="134"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -5032,21 +5045,21 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:18" ht="15" customHeight="1">
+    <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="90" t="s">
+      <c r="B18" s="80" t="s">
         <v>120</v>
       </c>
-      <c r="C18" s="96" t="s">
+      <c r="C18" s="144" t="s">
         <v>121</v>
       </c>
-      <c r="D18" s="97"/>
-      <c r="E18" s="96" t="s">
+      <c r="D18" s="112"/>
+      <c r="E18" s="144" t="s">
         <v>122</v>
       </c>
-      <c r="F18" s="107"/>
-      <c r="G18" s="107"/>
-      <c r="H18" s="97"/>
+      <c r="F18" s="111"/>
+      <c r="G18" s="111"/>
+      <c r="H18" s="112"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -5058,15 +5071,15 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="1:18" ht="15" customHeight="1">
+    <row r="19" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="91"/>
-      <c r="C19" s="98"/>
-      <c r="D19" s="99"/>
-      <c r="E19" s="130"/>
-      <c r="F19" s="107"/>
-      <c r="G19" s="107"/>
-      <c r="H19" s="97"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="145"/>
+      <c r="D19" s="146"/>
+      <c r="E19" s="142"/>
+      <c r="F19" s="111"/>
+      <c r="G19" s="111"/>
+      <c r="H19" s="112"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -5078,15 +5091,15 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:18" ht="15" customHeight="1">
+    <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="91"/>
-      <c r="C20" s="100"/>
-      <c r="D20" s="97"/>
-      <c r="E20" s="130"/>
-      <c r="F20" s="107"/>
-      <c r="G20" s="107"/>
-      <c r="H20" s="97"/>
+      <c r="B20" s="81"/>
+      <c r="C20" s="147"/>
+      <c r="D20" s="112"/>
+      <c r="E20" s="142"/>
+      <c r="F20" s="111"/>
+      <c r="G20" s="111"/>
+      <c r="H20" s="112"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -5098,15 +5111,15 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="1:18" ht="15" customHeight="1">
+    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="92"/>
-      <c r="C21" s="101"/>
-      <c r="D21" s="97"/>
-      <c r="E21" s="130"/>
-      <c r="F21" s="107"/>
-      <c r="G21" s="107"/>
-      <c r="H21" s="97"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="148"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="142"/>
+      <c r="F21" s="111"/>
+      <c r="G21" s="111"/>
+      <c r="H21" s="112"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -5118,15 +5131,15 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
+    <row r="22" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="93"/>
-      <c r="C22" s="102"/>
-      <c r="D22" s="103"/>
-      <c r="E22" s="131"/>
-      <c r="F22" s="132"/>
-      <c r="G22" s="132"/>
-      <c r="H22" s="103"/>
+      <c r="B22" s="83"/>
+      <c r="C22" s="149"/>
+      <c r="D22" s="115"/>
+      <c r="E22" s="143"/>
+      <c r="F22" s="114"/>
+      <c r="G22" s="114"/>
+      <c r="H22" s="115"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -5140,12 +5153,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B15:H15"/>
     <mergeCell ref="E21:H21"/>
     <mergeCell ref="E22:H22"/>
     <mergeCell ref="E19:H19"/>
@@ -5156,6 +5163,12 @@
     <mergeCell ref="E20:H20"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B15:H15"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -5174,16 +5187,16 @@
       <selection activeCell="B29" sqref="B29:B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.5" customWidth="1"/>
-    <col min="2" max="2" width="2.5" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="2.42578125" customWidth="1"/>
     <col min="3" max="3" width="76" customWidth="1"/>
-    <col min="4" max="4" width="82.5" customWidth="1"/>
-    <col min="5" max="14" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="82.42578125" customWidth="1"/>
+    <col min="5" max="14" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="12" customHeight="1">
+    <row r="1" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -5199,12 +5212,12 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1">
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="152" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="78"/>
+      <c r="C2" s="127"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -5217,12 +5230,12 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" ht="12" customHeight="1">
+    <row r="3" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="153" t="s">
         <v>124</v>
       </c>
-      <c r="C3" s="78"/>
+      <c r="C3" s="127"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -5235,7 +5248,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:14" ht="12" customHeight="1">
+    <row r="4" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -5251,13 +5264,13 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:14" ht="12" customHeight="1">
+    <row r="5" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="151" t="s">
         <v>125</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="127"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -5269,13 +5282,13 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:14" ht="12" customHeight="1">
+    <row r="6" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="83" t="s">
+      <c r="B6" s="151" t="s">
         <v>126</v>
       </c>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -5287,13 +5300,13 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" ht="12" customHeight="1">
+    <row r="7" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="82" t="s">
+      <c r="B7" s="150" t="s">
         <v>127</v>
       </c>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
+      <c r="C7" s="127"/>
+      <c r="D7" s="127"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -5305,7 +5318,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:14" ht="12" customHeight="1">
+    <row r="8" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="12"/>
       <c r="C8" s="11"/>
@@ -5321,7 +5334,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:14" ht="12" customHeight="1">
+    <row r="9" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -5337,7 +5350,7 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="1:14" ht="12.75" customHeight="1">
+    <row r="10" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="12" t="s">
         <v>128</v>
@@ -5355,7 +5368,7 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:14" ht="12.75" customHeight="1">
+    <row r="11" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="60"/>
       <c r="C11" s="61" t="s">
@@ -5375,7 +5388,7 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
     </row>
-    <row r="12" spans="1:14" ht="12" customHeight="1">
+    <row r="12" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="63">
         <v>1</v>
@@ -5397,7 +5410,7 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:14" ht="12" customHeight="1">
+    <row r="13" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="66">
         <f>B12+1</f>
@@ -5420,7 +5433,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:14" ht="12" customHeight="1">
+    <row r="14" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="66">
         <f>B13+1</f>
@@ -5443,7 +5456,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="1:14" ht="12" customHeight="1">
+    <row r="15" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="66">
         <f>B14+1</f>
@@ -5462,7 +5475,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
     </row>
-    <row r="16" spans="1:14" ht="12.75" customHeight="1">
+    <row r="16" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="70">
         <f>B15+1</f>
@@ -5481,7 +5494,7 @@
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
     </row>
-    <row r="17" spans="1:14" ht="12" customHeight="1">
+    <row r="17" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -5497,7 +5510,7 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
     </row>
-    <row r="18" spans="1:14" ht="12" customHeight="1">
+    <row r="18" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -5513,7 +5526,7 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
     </row>
-    <row r="19" spans="1:14" ht="12.75" customHeight="1">
+    <row r="19" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="12" t="s">
         <v>137</v>
@@ -5531,7 +5544,7 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
     </row>
-    <row r="20" spans="1:14" ht="12.75" customHeight="1">
+    <row r="20" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="60"/>
       <c r="C20" s="61" t="s">
@@ -5551,7 +5564,7 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
     </row>
-    <row r="21" spans="1:14" ht="12" customHeight="1">
+    <row r="21" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="63">
         <v>1</v>
@@ -5573,7 +5586,7 @@
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
     </row>
-    <row r="22" spans="1:14" ht="12" customHeight="1">
+    <row r="22" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="66">
         <f>B21+1</f>
@@ -5596,7 +5609,7 @@
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
     </row>
-    <row r="23" spans="1:14" ht="12" customHeight="1">
+    <row r="23" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="66">
         <f>B22+1</f>
@@ -5619,7 +5632,7 @@
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
     </row>
-    <row r="24" spans="1:14" ht="12" customHeight="1">
+    <row r="24" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="66">
         <f>B23+1</f>
@@ -5638,7 +5651,7 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="1:14" ht="12.75" customHeight="1">
+    <row r="25" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="70">
         <f>B24+1</f>
@@ -5657,7 +5670,7 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="1:14" ht="12" customHeight="1">
+    <row r="26" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -5673,7 +5686,7 @@
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="1:14" ht="12" customHeight="1">
+    <row r="27" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -5689,7 +5702,7 @@
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
     </row>
-    <row r="28" spans="1:14" ht="12.75" customHeight="1" thickBot="1">
+    <row r="28" spans="1:14" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="12" t="s">
         <v>146</v>
@@ -5707,13 +5720,13 @@
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
     </row>
-    <row r="29" spans="1:14" ht="12.75" customHeight="1">
+    <row r="29" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="127"/>
-      <c r="C29" s="120" t="s">
+      <c r="B29" s="99"/>
+      <c r="C29" s="92" t="s">
         <v>147</v>
       </c>
-      <c r="D29" s="121" t="s">
+      <c r="D29" s="93" t="s">
         <v>148</v>
       </c>
       <c r="E29" s="1"/>
@@ -5727,15 +5740,15 @@
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
     </row>
-    <row r="30" spans="1:14" ht="12" customHeight="1">
+    <row r="30" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="128">
+      <c r="B30" s="100">
         <v>1</v>
       </c>
-      <c r="C30" s="122" t="s">
+      <c r="C30" s="94" t="s">
         <v>149</v>
       </c>
-      <c r="D30" s="123" t="s">
+      <c r="D30" s="95" t="s">
         <v>150</v>
       </c>
       <c r="E30" s="1"/>
@@ -5749,16 +5762,16 @@
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
     </row>
-    <row r="31" spans="1:14" ht="12" customHeight="1">
+    <row r="31" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="128">
+      <c r="B31" s="100">
         <f>B30+1</f>
         <v>2</v>
       </c>
-      <c r="C31" s="122" t="s">
+      <c r="C31" s="94" t="s">
         <v>151</v>
       </c>
-      <c r="D31" s="124" t="s">
+      <c r="D31" s="96" t="s">
         <v>152</v>
       </c>
       <c r="E31" s="1"/>
@@ -5772,16 +5785,16 @@
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
     </row>
-    <row r="32" spans="1:14" ht="12" customHeight="1">
+    <row r="32" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="128">
+      <c r="B32" s="100">
         <f>B31+1</f>
         <v>3</v>
       </c>
-      <c r="C32" s="122" t="s">
+      <c r="C32" s="94" t="s">
         <v>153</v>
       </c>
-      <c r="D32" s="124" t="s">
+      <c r="D32" s="96" t="s">
         <v>154</v>
       </c>
       <c r="E32" s="1"/>
@@ -5795,16 +5808,16 @@
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
     </row>
-    <row r="33" spans="1:14" ht="12" customHeight="1">
+    <row r="33" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="128">
+      <c r="B33" s="100">
         <f>B32+1</f>
         <v>4</v>
       </c>
-      <c r="C33" s="122" t="s">
+      <c r="C33" s="94" t="s">
         <v>155</v>
       </c>
-      <c r="D33" s="124" t="s">
+      <c r="D33" s="96" t="s">
         <v>156</v>
       </c>
       <c r="E33" s="1"/>
@@ -5818,14 +5831,14 @@
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
     </row>
-    <row r="34" spans="1:14" ht="12.75" customHeight="1" thickBot="1">
+    <row r="34" spans="1:14" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
-      <c r="B34" s="129">
+      <c r="B34" s="101">
         <f>B33+1</f>
         <v>5</v>
       </c>
-      <c r="C34" s="125"/>
-      <c r="D34" s="126"/>
+      <c r="C34" s="97"/>
+      <c r="D34" s="98"/>
       <c r="E34" s="77"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>

</xml_diff>